<commit_message>
Updated count plan for 25Apr run
</commit_message>
<xml_diff>
--- a/Experiments/Activation/33MeVTa/CalibrationSources.xlsx
+++ b/Experiments/Activation/33MeVTa/CalibrationSources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>